<commit_message>
Included possibility of adding multiple columns for budget Now you can split your budget by, for example, Vendor and Country
 Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/dictionary/budget.xlsx
+++ b/dictionary/budget.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845F1A8C-D60A-4948-81D5-35BB15B6396B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1269C10-8420-4403-BE89-35E1796B5264}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7545" yWindow="3825" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6570" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Ad 4Game</t>
   </si>
@@ -35,6 +35,21 @@
   </si>
   <si>
     <t>Budget</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>us</t>
+  </si>
+  <si>
+    <t>br</t>
+  </si>
+  <si>
+    <t>ca</t>
+  </si>
+  <si>
+    <t>aunz</t>
   </si>
 </sst>
 </file>
@@ -352,43 +367,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
         <v>1500</v>
       </c>
     </row>

</xml_diff>